<commit_message>
Test Case File Changes
</commit_message>
<xml_diff>
--- a/TestCaseDocument/TestCases.xlsx
+++ b/TestCaseDocument/TestCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeltaXAssignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepository\TestCaseDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="122">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -448,6 +448,20 @@
   </si>
   <si>
     <t>TestCaseStatus</t>
+  </si>
+  <si>
+    <t>TC035</t>
+  </si>
+  <si>
+    <t>Validation of the acknowledgment email sent to the email id</t>
+  </si>
+  <si>
+    <t>1. Open the link in Browser
+2.Enter email field as 'saurabhsinghal001@gmail.com'
+3. Enter Submit Button</t>
+  </si>
+  <si>
+    <t>Email shold be delivered to the user</t>
   </si>
 </sst>
 </file>
@@ -823,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1538,8 +1552,23 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="7"/>
+    <row r="36" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="7"/>

</xml_diff>